<commit_message>
Implemented Highest Response Ratio Next and added results to Results.xlsx
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kittatamsaisaard/Google Drive/Third Year/Semester 2/Operating Systems/Assignments/Assignment 2/Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kittatamsaisaard/Documents/GitHub/Operataing-Systems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A7FFE6-9088-BC46-A896-904FF186C820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0469A420-94EF-ED48-9E27-A3A67A8C1324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{CF333519-F1B0-784E-846E-F88B6DF8763B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>total_wait_0</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Multilevel Feedback Queue Scheduling</t>
+  </si>
+  <si>
+    <t>Highest Response Ratio Next</t>
   </si>
 </sst>
 </file>
@@ -113,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -201,48 +204,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,24 +219,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{764F4EE7-E13F-4D48-A4AF-09D3994797A5}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,10 +588,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="2">
@@ -643,8 +611,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="13"/>
+      <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="4">
@@ -665,8 +633,8 @@
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="6">
@@ -686,30 +654,48 @@
       </c>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="17" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="11">
         <v>7746</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="11">
         <v>14675</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="11">
         <v>22421</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="11">
         <v>739</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="14">
         <v>68</v>
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
+    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="18">
+        <v>6488</v>
+      </c>
+      <c r="D6" s="18">
+        <v>5354</v>
+      </c>
+      <c r="E6" s="18">
+        <v>11842</v>
+      </c>
+      <c r="F6" s="18">
+        <v>1000</v>
+      </c>
+      <c r="G6" s="19">
+        <v>51</v>
+      </c>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -717,10 +703,10 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2">
@@ -741,8 +727,8 @@
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="13"/>
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="4">
@@ -763,8 +749,8 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="6">
@@ -784,41 +770,58 @@
       </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="8" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="13"/>
+      <c r="B11" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="11">
         <v>6405</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="11">
         <v>18135</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="11">
         <v>24540</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="11">
         <v>754</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="14">
         <v>70</v>
       </c>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
+    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="18">
+        <v>6855</v>
+      </c>
+      <c r="D12" s="18">
+        <v>7267</v>
+      </c>
+      <c r="E12" s="18">
+        <v>14122</v>
+      </c>
+      <c r="F12" s="18">
+        <v>1123</v>
+      </c>
+      <c r="G12" s="19">
+        <v>52</v>
+      </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="2">
@@ -839,8 +842,8 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="13"/>
+      <c r="B15" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="4">
@@ -861,8 +864,8 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="13"/>
+      <c r="B16" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="6">
@@ -881,44 +884,59 @@
         <v>398</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="8" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="13"/>
+      <c r="B17" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="11">
         <v>12909</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="11">
         <v>22199</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="11">
         <v>35108</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="11">
         <v>896</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="14">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="16"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
+    <row r="18" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="18">
+        <v>12973</v>
+      </c>
+      <c r="D18" s="18">
+        <v>7600</v>
+      </c>
+      <c r="E18" s="18">
+        <v>20573</v>
+      </c>
+      <c r="F18" s="18">
+        <v>1370</v>
+      </c>
+      <c r="G18" s="19">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A14:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added final scheduler results
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kittatamsaisaard/Documents/GitHub/Operataing-Systems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0469A420-94EF-ED48-9E27-A3A67A8C1324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D61245-8F9A-D04E-8B94-6C86855E872C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{CF333519-F1B0-784E-846E-F88B6DF8763B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>total_wait_0</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Highest Response Ratio Next</t>
+  </si>
+  <si>
+    <t>SRTF + Aging + MFQS + PS /w RR + More</t>
   </si>
 </sst>
 </file>
@@ -125,10 +128,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -138,37 +150,6 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -199,46 +180,72 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{764F4EE7-E13F-4D48-A4AF-09D3994797A5}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -588,10 +595,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="2">
@@ -611,8 +618,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="4">
@@ -633,8 +640,8 @@
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="6">
@@ -655,20 +662,20 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="16" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="13">
         <v>7746</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="13">
         <v>14675</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="13">
         <v>22421</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="13">
         <v>739</v>
       </c>
       <c r="G5" s="14">
@@ -676,267 +683,326 @@
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="17" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="6">
         <v>6488</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="6">
         <v>5354</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="6">
         <v>11842</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="6">
         <v>1000</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="7">
         <v>51</v>
       </c>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="16">
+        <v>8385</v>
+      </c>
+      <c r="D7" s="16">
+        <v>15037</v>
+      </c>
+      <c r="E7" s="16">
+        <v>23422</v>
+      </c>
+      <c r="F7" s="16">
+        <v>182</v>
+      </c>
+      <c r="G7" s="17">
+        <v>108</v>
+      </c>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C9" s="2">
         <v>13661</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D9" s="2">
         <v>14023</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E9" s="2">
         <v>27684</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F9" s="2">
         <v>292</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G9" s="3">
         <v>201</v>
       </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="9" t="s">
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C10" s="4">
         <v>6786</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D10" s="4">
         <v>6513</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E10" s="4">
         <v>13299</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F10" s="4">
         <v>1263</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G10" s="5">
         <v>56</v>
       </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="9" t="s">
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C11" s="6">
         <v>5350</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D11" s="6">
         <v>22682</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E11" s="6">
         <v>28032</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F11" s="6">
         <v>648</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G11" s="7">
         <v>368</v>
       </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="16" t="s">
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="11"/>
+      <c r="B12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C12" s="13">
         <v>6405</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D12" s="13">
         <v>18135</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E12" s="13">
         <v>24540</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F12" s="13">
         <v>754</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G12" s="14">
         <v>70</v>
       </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="17" t="s">
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
+      <c r="B13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C13" s="6">
         <v>6855</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D13" s="6">
         <v>7267</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E13" s="6">
         <v>14122</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F13" s="6">
         <v>1123</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G13" s="7">
         <v>52</v>
       </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+    <row r="14" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="16">
+        <v>7158</v>
+      </c>
+      <c r="D14" s="16">
+        <v>17481</v>
+      </c>
+      <c r="E14" s="16">
+        <v>24639</v>
+      </c>
+      <c r="F14" s="16">
+        <v>26</v>
+      </c>
+      <c r="G14" s="17">
+        <v>120</v>
+      </c>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C16" s="2">
         <v>22084</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D16" s="2">
         <v>16943</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E16" s="2">
         <v>39027</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F16" s="2">
         <v>354</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G16" s="3">
         <v>225</v>
       </c>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="9" t="s">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="11"/>
+      <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C17" s="4">
         <v>11134</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D17" s="4">
         <v>7093</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E17" s="4">
         <v>18227</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F17" s="4">
         <v>1415</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G17" s="5">
         <v>57</v>
       </c>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="9" t="s">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="11"/>
+      <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C18" s="6">
         <v>13200</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D18" s="6">
         <v>27624</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E18" s="6">
         <v>40824</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F18" s="6">
         <v>1005</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G18" s="7">
         <v>398</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="16" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="11"/>
+      <c r="B19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C19" s="13">
         <v>12909</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D19" s="13">
         <v>22199</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E19" s="13">
         <v>35108</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F19" s="13">
         <v>896</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G19" s="14">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="17" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="11"/>
+      <c r="B20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C20" s="6">
         <v>12973</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D20" s="6">
         <v>7600</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E20" s="6">
         <v>20573</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F20" s="6">
         <v>1370</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G20" s="7">
         <v>51</v>
       </c>
     </row>
+    <row r="21" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="16">
+        <v>12309</v>
+      </c>
+      <c r="D21" s="16">
+        <v>23687</v>
+      </c>
+      <c r="E21" s="16">
+        <v>35996</v>
+      </c>
+      <c r="F21" s="16">
+        <v>65</v>
+      </c>
+      <c r="G21" s="17">
+        <v>129</v>
+      </c>
+    </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
+      <c r="A23" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A16:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updated Final Scheduler and Results Spreadsheet
The Final Scheduler has been improved upon to reduce the longest response time.

Long response times occur when customers arrive in at the same time and the customer that arrives at the next time interval has to wait a very long time in order to start playing.
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kittatamsaisaard/Documents/GitHub/Operataing-Systems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D61245-8F9A-D04E-8B94-6C86855E872C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42412EAB-ABA7-D441-AEF4-88A7C7036943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{CF333519-F1B0-784E-846E-F88B6DF8763B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>total_wait_0</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>SRTF + Aging + MFQS + PS /w RR + More</t>
+  </si>
+  <si>
+    <t>Superior Scheduler</t>
   </si>
 </sst>
 </file>
@@ -105,7 +108,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,8 +121,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -213,25 +222,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -241,11 +277,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{764F4EE7-E13F-4D48-A4AF-09D3994797A5}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,7 +620,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
+      <c r="A1" s="2"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,414 +638,468 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="13">
         <v>12972</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="13">
         <v>10606</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="13">
         <v>23578</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="13">
         <v>266</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="14">
         <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="12">
+        <v>4119</v>
+      </c>
+      <c r="D3" s="11">
+        <v>16490</v>
+      </c>
+      <c r="E3" s="11">
+        <v>20609</v>
+      </c>
+      <c r="F3" s="11">
+        <v>2</v>
+      </c>
+      <c r="G3" s="17">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="9"/>
+      <c r="B4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C4" s="2">
         <v>5676</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D4" s="2">
         <v>5485</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E4" s="2">
         <v>11161</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F4" s="2">
         <v>1133</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G4" s="3">
         <v>58</v>
       </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="4" t="s">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="9"/>
+      <c r="B5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C5" s="4">
         <v>5895</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D5" s="4">
         <v>19238</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E5" s="4">
         <v>25133</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F5" s="4">
         <v>668</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G5" s="5">
         <v>330</v>
       </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="9" t="s">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="9"/>
+      <c r="B6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C6" s="6">
         <v>7746</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D6" s="6">
         <v>14675</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E6" s="6">
         <v>22421</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F6" s="6">
         <v>739</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G6" s="7">
         <v>68</v>
       </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="9" t="s">
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="9"/>
+      <c r="B7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C7" s="4">
         <v>6488</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D7" s="4">
         <v>5354</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E7" s="4">
         <v>11842</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F7" s="4">
         <v>1000</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G7" s="5">
         <v>51</v>
       </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="15" t="s">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C8" s="21">
         <v>8385</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D8" s="21">
         <v>15037</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E8" s="21">
         <v>23422</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F8" s="21">
         <v>182</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G8" s="22">
         <v>108</v>
       </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C10" s="13">
         <v>13661</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D10" s="13">
         <v>14023</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E10" s="13">
         <v>27684</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F10" s="13">
         <v>292</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G10" s="14">
         <v>201</v>
       </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="4" t="s">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="9"/>
+      <c r="B11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="12">
+        <v>4389</v>
+      </c>
+      <c r="D11" s="11">
+        <v>17044</v>
+      </c>
+      <c r="E11" s="11">
+        <v>21433</v>
+      </c>
+      <c r="F11" s="11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="17">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="9"/>
+      <c r="B12" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C12" s="2">
         <v>6786</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D12" s="2">
         <v>6513</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E12" s="2">
         <v>13299</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F12" s="2">
         <v>1263</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G12" s="3">
         <v>56</v>
       </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-      <c r="B11" s="4" t="s">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
+      <c r="B13" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C13" s="4">
         <v>5350</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D13" s="4">
         <v>22682</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E13" s="4">
         <v>28032</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F13" s="4">
         <v>648</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G13" s="5">
         <v>368</v>
       </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
-      <c r="B12" s="9" t="s">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="9"/>
+      <c r="B14" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C14" s="6">
         <v>6405</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D14" s="6">
         <v>18135</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E14" s="6">
         <v>24540</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F14" s="6">
         <v>754</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G14" s="7">
         <v>70</v>
       </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="9" t="s">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C15" s="4">
         <v>6855</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D15" s="4">
         <v>7267</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E15" s="4">
         <v>14122</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F15" s="4">
         <v>1123</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G15" s="5">
         <v>52</v>
       </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="15" t="s">
+    </row>
+    <row r="16" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C16" s="21">
         <v>7158</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D16" s="21">
         <v>17481</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E16" s="21">
         <v>24639</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F16" s="21">
         <v>26</v>
       </c>
-      <c r="G14" s="17">
+      <c r="G16" s="22">
         <v>120</v>
       </c>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+    </row>
+    <row r="17" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B18" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C18" s="13">
         <v>22084</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D18" s="13">
         <v>16943</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E18" s="13">
         <v>39027</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F18" s="13">
         <v>354</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G18" s="14">
         <v>225</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="4" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="9"/>
+      <c r="B19" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="12">
+        <v>7559</v>
+      </c>
+      <c r="D19" s="11">
+        <v>25013</v>
+      </c>
+      <c r="E19" s="11">
+        <v>32572</v>
+      </c>
+      <c r="F19" s="11">
+        <v>2</v>
+      </c>
+      <c r="G19" s="17">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="9"/>
+      <c r="B20" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C20" s="2">
         <v>11134</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D20" s="2">
         <v>7093</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E20" s="2">
         <v>18227</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F20" s="2">
         <v>1415</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G20" s="3">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-      <c r="B18" s="4" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="9"/>
+      <c r="B21" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C21" s="4">
         <v>13200</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D21" s="4">
         <v>27624</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E21" s="4">
         <v>40824</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F21" s="4">
         <v>1005</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G21" s="5">
         <v>398</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="9" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="9"/>
+      <c r="B22" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C22" s="6">
         <v>12909</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D22" s="6">
         <v>22199</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E22" s="6">
         <v>35108</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F22" s="6">
         <v>896</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G22" s="7">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-      <c r="B20" s="9" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="9"/>
+      <c r="B23" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C23" s="4">
         <v>12973</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D23" s="4">
         <v>7600</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E23" s="4">
         <v>20573</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F23" s="4">
         <v>1370</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G23" s="5">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="15" t="s">
+    <row r="24" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C24" s="21">
         <v>12309</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D24" s="21">
         <v>23687</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E24" s="21">
         <v>35996</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F24" s="21">
         <v>65</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G24" s="22">
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
-    </row>
+    <row r="33" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A18:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>